<commit_message>
Query and clients added
</commit_message>
<xml_diff>
--- a/DailyPricingAutomationTest/config/Clients.xlsx
+++ b/DailyPricingAutomationTest/config/Clients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ankit-WorkArea-Automation\GithubProjects\GitWorkspace_i2o_Dailyfeed\DailyPricingAutomationTest\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBDB424-1950-4D64-BC4C-4B7BD37B78B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536AF70D-114A-460C-B0D7-CC9818D527EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Execution status</t>
   </si>
@@ -54,10 +54,25 @@
     <t>i2o-dev-jvc</t>
   </si>
   <si>
+    <t>i2o-dev-30watt</t>
+  </si>
+  <si>
+    <t>i2o-dev-ossur</t>
+  </si>
+  <si>
+    <t>i2o-dev-ffl</t>
+  </si>
+  <si>
+    <t>i2o-preprod-mycharge</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>i2o-dev-30watt</t>
+    <t>i2o-preprod-interaxon</t>
+  </si>
+  <si>
+    <t>i2o-preprod-talkworks</t>
   </si>
   <si>
     <t>Yes</t>
@@ -467,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +539,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,15 +547,55 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>